<commit_message>
export excel, backup, import
</commit_message>
<xml_diff>
--- a/back-end/all_members_data.xlsx
+++ b/back-end/all_members_data.xlsx
@@ -4,13 +4,105 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="Family Member Data" state="visible" r:id="rId3"/>
-    <sheet sheetId="2" name="Education Data" state="visible" r:id="rId4"/>
-    <sheet sheetId="3" name="Job Data" state="visible" r:id="rId5"/>
-    <sheet sheetId="4" name="Contact Data" state="visible" r:id="rId6"/>
+    <sheet sheetId="1" name="Family Member Data" state="visible" r:id="rId4"/>
+    <sheet sheetId="2" name="Education Data" state="visible" r:id="rId5"/>
+    <sheet sheetId="3" name="Job Data" state="visible" r:id="rId6"/>
+    <sheet sheetId="4" name="Contact Data" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
+  <si>
+    <t>MemberID</t>
+  </si>
+  <si>
+    <t>FatherID</t>
+  </si>
+  <si>
+    <t>MotherID</t>
+  </si>
+  <si>
+    <t>MemberName</t>
+  </si>
+  <si>
+    <t>NickName</t>
+  </si>
+  <si>
+    <t>BirthOrder</t>
+  </si>
+  <si>
+    <t>Origin</t>
+  </si>
+  <si>
+    <t>NationalityID</t>
+  </si>
+  <si>
+    <t>ReligionID</t>
+  </si>
+  <si>
+    <t>Dob</t>
+  </si>
+  <si>
+    <t>LunarDob</t>
+  </si>
+  <si>
+    <t>BirthPlace</t>
+  </si>
+  <si>
+    <t>IsDead</t>
+  </si>
+  <si>
+    <t>Dod</t>
+  </si>
+  <si>
+    <t>LunarDod</t>
+  </si>
+  <si>
+    <t>PlaceOfDeath</t>
+  </si>
+  <si>
+    <t>GraveSite</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>Generation</t>
+  </si>
+  <si>
+    <t>BloodType</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>CodeID</t>
+  </si>
+  <si>
+    <t>Image</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>962359</t>
+  </si>
+  <si>
+    <t>ff</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>hh</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -385,9 +477,233 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:W5"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>853</v>
+      </c>
+      <c r="B2">
+        <v>836</v>
+      </c>
+      <c r="C2">
+        <v>889</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>4</v>
+      </c>
+      <c r="U2">
+        <v>1</v>
+      </c>
+      <c r="V2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>862</v>
+      </c>
+      <c r="B3">
+        <v>853</v>
+      </c>
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>5</v>
+      </c>
+      <c r="U3">
+        <v>1</v>
+      </c>
+      <c r="V3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>873</v>
+      </c>
+      <c r="B4">
+        <v>862</v>
+      </c>
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>6</v>
+      </c>
+      <c r="U4">
+        <v>1</v>
+      </c>
+      <c r="V4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>889</v>
+      </c>
+      <c r="D5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>3</v>
+      </c>
+      <c r="U5">
+        <v>0</v>
+      </c>
+      <c r="V5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>

</xml_diff>